<commit_message>
Phân chi công việc
</commit_message>
<xml_diff>
--- a/KeHoachThucHien.xlsx
+++ b/KeHoachThucHien.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Courses\book_tour\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBDAB70-C952-48EB-B60F-04B570D45073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1359AB8D-B2B0-4429-A4C6-7260BEE2E33B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15720" xr2:uid="{F4581A85-E430-4ED3-97EB-B987101897CE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F4581A85-E430-4ED3-97EB-B987101897CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="89">
   <si>
     <t>KHOA ĐÀO TẠO CHẤT LƯỢNG CAO</t>
   </si>
@@ -220,9 +220,6 @@
     <t>30/10/2022</t>
   </si>
   <si>
-    <t xml:space="preserve">Trang các tour du lịch </t>
-  </si>
-  <si>
     <t>Trang chủ (hiển thị các tour du lịch nổi bật, có giá ưu đãi giảm giá)</t>
   </si>
   <si>
@@ -302,6 +299,9 @@
   </si>
   <si>
     <t>Làm powerpoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trang search tour du lịch </t>
   </si>
 </sst>
 </file>
@@ -371,6 +371,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -389,37 +396,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -593,6 +574,25 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -643,19 +643,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2625AEDE-7ABE-4A4E-9C5A-6E0D4CCC3E1E}" name="Table7" displayName="Table7" ref="A10:J47" totalsRowShown="0" headerRowDxfId="11" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2625AEDE-7ABE-4A4E-9C5A-6E0D4CCC3E1E}" name="Table7" displayName="Table7" ref="A10:J47" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A10:J47" xr:uid="{2625AEDE-7ABE-4A4E-9C5A-6E0D4CCC3E1E}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{9935C1E0-CE72-4646-8D1C-04C71EC9E079}" name="1" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{B9239D8B-1976-454F-9BD9-506EEE752E62}" name="Công việc" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{3ECBC3CF-F360-42E3-82EF-CE73E1AA94D4}" name="Chi tiết công việc" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{73B5385A-485E-4019-845E-AFA4C38FC7B9}" name="Hồ Quốc Vinh" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{793CFA4D-3A13-487C-B2BC-51E5DF31F0B2}" name="Trịnh Đinh Hoàng Huy" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{F2DF50AA-E8F9-47F9-AB20-ECBD1EA36C1F}" name="Ngày bắt đầu dự kiến" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{F6D2A759-7FE4-4702-8FE4-78DF2A5CEC9E}" name="Ngày kết thúc dự kiến" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{874399A5-12DF-4A6B-9624-59AD7572FC19}" name="Ngày bắt đầu thực tế" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{7FD2D243-2310-40DD-A294-E6586F752E24}" name="Ngày kết thúc thực tế" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{11CCCA66-700F-43A1-8E0C-688D5716BC56}" name="Ghi chú" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{9935C1E0-CE72-4646-8D1C-04C71EC9E079}" name="1" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{B9239D8B-1976-454F-9BD9-506EEE752E62}" name="Công việc" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{3ECBC3CF-F360-42E3-82EF-CE73E1AA94D4}" name="Chi tiết công việc" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{73B5385A-485E-4019-845E-AFA4C38FC7B9}" name="Hồ Quốc Vinh" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{793CFA4D-3A13-487C-B2BC-51E5DF31F0B2}" name="Trịnh Đinh Hoàng Huy" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{F2DF50AA-E8F9-47F9-AB20-ECBD1EA36C1F}" name="Ngày bắt đầu dự kiến" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{F6D2A759-7FE4-4702-8FE4-78DF2A5CEC9E}" name="Ngày kết thúc dự kiến" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{874399A5-12DF-4A6B-9624-59AD7572FC19}" name="Ngày bắt đầu thực tế" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{7FD2D243-2310-40DD-A294-E6586F752E24}" name="Ngày kết thúc thực tế" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{11CCCA66-700F-43A1-8E0C-688D5716BC56}" name="Ghi chú" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -960,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90171A7B-7F7B-4202-8410-7C81B775AF4A}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -980,86 +980,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
@@ -1075,7 +1075,7 @@
     </row>
     <row r="10" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>3</v>
@@ -1112,12 +1112,10 @@
       <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1130,7 +1128,7 @@
       <c r="H11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="5">
         <v>44570</v>
       </c>
       <c r="J11" s="2"/>
@@ -1138,21 +1136,19 @@
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="11">
+      <c r="H12" s="5">
         <v>44601</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="5">
         <v>44629</v>
       </c>
       <c r="J12" s="2"/>
@@ -1160,7 +1156,7 @@
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="6" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -1171,10 +1167,10 @@
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="11">
+      <c r="H13" s="5">
         <v>44660</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="5">
         <v>44690</v>
       </c>
       <c r="J13" s="2"/>
@@ -1186,21 +1182,19 @@
       <c r="B14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="11">
+      <c r="H14" s="5">
         <v>44721</v>
       </c>
-      <c r="I14" s="11">
+      <c r="I14" s="5">
         <v>44782</v>
       </c>
       <c r="J14" s="2"/>
@@ -1208,21 +1202,19 @@
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="11">
+      <c r="H15" s="5">
         <v>44813</v>
       </c>
-      <c r="I15" s="11">
+      <c r="I15" s="5">
         <v>44843</v>
       </c>
       <c r="J15" s="2"/>
@@ -1230,7 +1222,7 @@
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="6" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -1241,10 +1233,10 @@
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="11">
+      <c r="H16" s="5">
         <v>44874</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="5">
         <v>44904</v>
       </c>
       <c r="J16" s="2"/>
@@ -1252,7 +1244,7 @@
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -1278,7 +1270,7 @@
       <c r="B18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -1304,7 +1296,7 @@
       <c r="B19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -1330,7 +1322,7 @@
       <c r="B20" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -1344,7 +1336,7 @@
       <c r="H20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I20" s="11">
+      <c r="I20" s="5">
         <v>44630</v>
       </c>
       <c r="J20" s="2"/>
@@ -1352,21 +1344,19 @@
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="11">
+      <c r="H21" s="5">
         <v>44661</v>
       </c>
-      <c r="I21" s="11">
+      <c r="I21" s="5">
         <v>44661</v>
       </c>
       <c r="J21" s="2"/>
@@ -1374,21 +1364,19 @@
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="7" t="s">
         <v>39</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="11">
+      <c r="H22" s="5">
         <v>44691</v>
       </c>
-      <c r="I22" s="11">
+      <c r="I22" s="5">
         <v>44691</v>
       </c>
       <c r="J22" s="2"/>
@@ -1396,21 +1384,19 @@
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="11">
+      <c r="H23" s="5">
         <v>44722</v>
       </c>
-      <c r="I23" s="11">
+      <c r="I23" s="5">
         <v>44783</v>
       </c>
       <c r="J23" s="2"/>
@@ -1418,21 +1404,19 @@
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="7" t="s">
         <v>41</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="11">
+      <c r="H24" s="5">
         <v>44844</v>
       </c>
-      <c r="I24" s="11">
+      <c r="I24" s="5">
         <v>44905</v>
       </c>
       <c r="J24" s="2"/>
@@ -1440,18 +1424,16 @@
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="D25" s="2"/>
       <c r="E25" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="11">
+      <c r="H25" s="5">
         <v>44905</v>
       </c>
       <c r="I25" s="2" t="s">
@@ -1462,15 +1444,13 @@
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="7" t="s">
         <v>44</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2" t="s">
@@ -1484,12 +1464,10 @@
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
         <v>14</v>
       </c>
@@ -1506,15 +1484,13 @@
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="7" t="s">
         <v>50</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2" t="s">
@@ -1528,12 +1504,10 @@
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
         <v>14</v>
       </c>
@@ -1550,15 +1524,13 @@
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="7" t="s">
         <v>55</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2" t="s">
@@ -1576,8 +1548,8 @@
       <c r="B31" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="13" t="s">
-        <v>62</v>
+      <c r="C31" s="7" t="s">
+        <v>61</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>14</v>
@@ -1598,21 +1570,19 @@
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="C32" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I32" s="11">
+        <v>62</v>
+      </c>
+      <c r="I32" s="5">
         <v>44572</v>
       </c>
       <c r="J32" s="2"/>
@@ -1620,21 +1590,19 @@
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
-      <c r="C33" s="13" t="s">
-        <v>64</v>
+      <c r="C33" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
-      <c r="H33" s="11">
+      <c r="H33" s="5">
         <v>44603</v>
       </c>
-      <c r="I33" s="11">
+      <c r="I33" s="5">
         <v>44631</v>
       </c>
       <c r="J33" s="2"/>
@@ -1642,21 +1610,19 @@
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="C34" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" s="2"/>
       <c r="E34" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="11">
+      <c r="H34" s="5">
         <v>44662</v>
       </c>
-      <c r="I34" s="11">
+      <c r="I34" s="5">
         <v>44662</v>
       </c>
       <c r="J34" s="2"/>
@@ -1664,21 +1630,19 @@
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
-      <c r="C35" s="13" t="s">
-        <v>67</v>
+      <c r="C35" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="11">
+      <c r="H35" s="5">
         <v>44692</v>
       </c>
-      <c r="I35" s="11">
+      <c r="I35" s="5">
         <v>44692</v>
       </c>
       <c r="J35" s="2"/>
@@ -1686,21 +1650,19 @@
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
-      <c r="C36" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="C36" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" s="2"/>
       <c r="E36" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="11">
+      <c r="H36" s="5">
         <v>44723</v>
       </c>
-      <c r="I36" s="11">
+      <c r="I36" s="5">
         <v>44723</v>
       </c>
       <c r="J36" s="2"/>
@@ -1708,21 +1670,19 @@
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
-      <c r="C37" s="13" t="s">
-        <v>69</v>
+      <c r="C37" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
-      <c r="H37" s="11">
+      <c r="H37" s="5">
         <v>44753</v>
       </c>
-      <c r="I37" s="11">
+      <c r="I37" s="5">
         <v>44753</v>
       </c>
       <c r="J37" s="2"/>
@@ -1730,21 +1690,19 @@
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
-      <c r="C38" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="C38" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D38" s="2"/>
       <c r="E38" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
-      <c r="H38" s="11">
+      <c r="H38" s="5">
         <v>44784</v>
       </c>
-      <c r="I38" s="11">
+      <c r="I38" s="5">
         <v>44784</v>
       </c>
       <c r="J38" s="2"/>
@@ -1752,21 +1710,19 @@
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
-      <c r="C39" s="13" t="s">
-        <v>71</v>
+      <c r="C39" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
-      <c r="H39" s="11">
+      <c r="H39" s="5">
         <v>44815</v>
       </c>
-      <c r="I39" s="11">
+      <c r="I39" s="5">
         <v>44815</v>
       </c>
       <c r="J39" s="2"/>
@@ -1774,21 +1730,19 @@
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
-      <c r="C40" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="C40" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D40" s="2"/>
       <c r="E40" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
-      <c r="H40" s="11">
+      <c r="H40" s="5">
         <v>44845</v>
       </c>
-      <c r="I40" s="11">
+      <c r="I40" s="5">
         <v>44845</v>
       </c>
       <c r="J40" s="2"/>
@@ -1796,21 +1750,19 @@
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
-      <c r="C41" s="13" t="s">
-        <v>73</v>
+      <c r="C41" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
-      <c r="H41" s="11">
+      <c r="H41" s="5">
         <v>44876</v>
       </c>
-      <c r="I41" s="11">
+      <c r="I41" s="5">
         <v>44876</v>
       </c>
       <c r="J41" s="2"/>
@@ -1820,32 +1772,30 @@
         <v>7</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C42" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="D42" s="2"/>
       <c r="E42" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
-      <c r="H42" s="11">
+      <c r="H42" s="5">
         <v>44906</v>
       </c>
-      <c r="I42" s="11" t="s">
-        <v>80</v>
+      <c r="I42" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="J42" s="2"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
-      <c r="C43" s="13" t="s">
-        <v>76</v>
+      <c r="C43" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>14</v>
@@ -1856,10 +1806,10 @@
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I43" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="J43" s="2"/>
     </row>
@@ -1868,10 +1818,10 @@
         <v>8</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C44" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>78</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>14</v>
@@ -1882,18 +1832,18 @@
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I44" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="J44" s="2"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
-      <c r="C45" s="13" t="s">
-        <v>79</v>
+      <c r="C45" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>14</v>
@@ -1904,10 +1854,10 @@
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J45" s="2"/>
     </row>
@@ -1916,10 +1866,10 @@
         <v>9</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>14</v>
@@ -1929,10 +1879,10 @@
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
-      <c r="H46" s="11">
+      <c r="H46" s="5">
         <v>44573</v>
       </c>
-      <c r="I46" s="11">
+      <c r="I46" s="5">
         <v>44663</v>
       </c>
       <c r="J46" s="2"/>
@@ -1940,8 +1890,8 @@
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
-      <c r="C47" s="2" t="s">
-        <v>88</v>
+      <c r="C47" s="7" t="s">
+        <v>87</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>14</v>
@@ -1951,10 +1901,10 @@
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
-      <c r="H47" s="11">
+      <c r="H47" s="5">
         <v>44693</v>
       </c>
-      <c r="I47" s="11">
+      <c r="I47" s="5">
         <v>44724</v>
       </c>
       <c r="J47" s="2"/>

</xml_diff>